<commit_message>
added tests for snapdeal
</commit_message>
<xml_diff>
--- a/SeleniumTestProject/src/main/resources/testData/SampleTestData.xlsx
+++ b/SeleniumTestProject/src/main/resources/testData/SampleTestData.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -24,12 +29,6 @@
     <t>SearchData</t>
   </si>
   <si>
-    <t>cooking</t>
-  </si>
-  <si>
-    <t>obama</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -37,6 +36,12 @@
   </si>
   <si>
     <t>Arvind</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>pen</t>
   </si>
 </sst>
 </file>
@@ -378,15 +383,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,33 +399,38 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -430,9 +440,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -442,8 +457,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>